<commit_message>
Updated data tables to fix error in Woods 2017
</commit_message>
<xml_diff>
--- a/datatables/Wood 2017 Human Clint and CLh.xlsx
+++ b/datatables/Wood 2017 Human Clint and CLh.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwambaug\git\httkdatatables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwambaug\git\httk-dev\datatables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61CEC9E3-66D3-4516-94AE-7AD60C5317A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F8C76C0-61A3-460F-81F1-AFFA7718A7BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2574,20 +2574,20 @@
   <dimension ref="A1:O119"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2:O119"/>
+      <selection activeCell="O3" sqref="O3:O119"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.7265625" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" customWidth="1"/>
+    <col min="5" max="5" width="12.453125" customWidth="1"/>
     <col min="7" max="7" width="12" customWidth="1"/>
-    <col min="15" max="15" width="13.5703125" customWidth="1"/>
+    <col min="15" max="15" width="13.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>645</v>
       </c>
@@ -2634,7 +2634,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="30" t="s">
         <v>528</v>
       </c>
@@ -2672,11 +2672,11 @@
       <c r="M2" s="6"/>
       <c r="N2" s="6"/>
       <c r="O2" s="33">
-        <f>K2/120/21.4*1000</f>
+        <f>IF(NOT(ISBLANK(K2)),K2/120/21.4*1000,"")</f>
         <v>1.985981308411215</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="23" x14ac:dyDescent="0.35">
       <c r="A3" s="30" t="s">
         <v>529</v>
       </c>
@@ -2720,11 +2720,11 @@
         <v>12</v>
       </c>
       <c r="O3" s="33">
-        <f t="shared" ref="O3:O66" si="0">K3/120/21.4*1000</f>
+        <f t="shared" ref="O3:O66" si="0">IF(NOT(ISBLANK(K3)),K3/120/21.4*1000,"")</f>
         <v>1.0903426791277258</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="23" x14ac:dyDescent="0.35">
       <c r="A4" s="30" t="s">
         <v>530</v>
       </c>
@@ -2759,12 +2759,12 @@
       <c r="N4" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="O4" s="33">
+      <c r="O4" s="33" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" ht="24" x14ac:dyDescent="0.25">
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="23" x14ac:dyDescent="0.35">
       <c r="A5" s="30" t="s">
         <v>531</v>
       </c>
@@ -2812,7 +2812,7 @@
         <v>0.38940809968847356</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" s="30" t="s">
         <v>532</v>
       </c>
@@ -2860,7 +2860,7 @@
         <v>22.975077881619935</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" ht="23" x14ac:dyDescent="0.35">
       <c r="A7" s="31" t="s">
         <v>533</v>
       </c>
@@ -2908,7 +2908,7 @@
         <v>12.461059190031154</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" s="30" t="s">
         <v>534</v>
       </c>
@@ -2943,12 +2943,12 @@
       <c r="N8" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="O8" s="33">
+      <c r="O8" s="33" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" s="30" t="s">
         <v>535</v>
       </c>
@@ -2996,7 +2996,7 @@
         <v>0.50623052959501558</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" s="30" t="s">
         <v>536</v>
       </c>
@@ -3044,7 +3044,7 @@
         <v>1.985981308411215</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" s="30" t="s">
         <v>537</v>
       </c>
@@ -3079,12 +3079,12 @@
       <c r="N11" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="O11" s="33">
+      <c r="O11" s="33" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" s="30" t="s">
         <v>538</v>
       </c>
@@ -3132,7 +3132,7 @@
         <v>2.1417445482866042</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13" s="30" t="s">
         <v>539</v>
       </c>
@@ -3180,7 +3180,7 @@
         <v>2.3364485981308416</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" ht="23" x14ac:dyDescent="0.35">
       <c r="A14" s="30" t="s">
         <v>540</v>
       </c>
@@ -3228,7 +3228,7 @@
         <v>13.2398753894081</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" ht="23" x14ac:dyDescent="0.35">
       <c r="A15" s="30" t="s">
         <v>541</v>
       </c>
@@ -3276,7 +3276,7 @@
         <v>30.373831775700939</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" ht="23" x14ac:dyDescent="0.35">
       <c r="A16" s="30" t="s">
         <v>542</v>
       </c>
@@ -3324,7 +3324,7 @@
         <v>2.0638629283489101</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A17" s="30" t="s">
         <v>543</v>
       </c>
@@ -3366,7 +3366,7 @@
         <v>2.3753894080996885</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A18" s="30" t="s">
         <v>544</v>
       </c>
@@ -3414,7 +3414,7 @@
         <v>98.520249221183818</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="24" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A19" s="30" t="s">
         <v>545</v>
       </c>
@@ -3456,7 +3456,7 @@
         <v>2.8816199376947043</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="36" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A20" s="30" t="s">
         <v>546</v>
       </c>
@@ -3504,7 +3504,7 @@
         <v>195.09345794392524</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="24" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" ht="23" x14ac:dyDescent="0.35">
       <c r="A21" s="30" t="s">
         <v>547</v>
       </c>
@@ -3552,7 +3552,7 @@
         <v>5.4517133956386301</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="36" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A22" s="30" t="s">
         <v>548</v>
       </c>
@@ -3600,7 +3600,7 @@
         <v>8.5669781931464168</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A23" s="30" t="s">
         <v>549</v>
       </c>
@@ -3642,7 +3642,7 @@
         <v>24.532710280373834</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="24" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" ht="23" x14ac:dyDescent="0.35">
       <c r="A24" s="30" t="s">
         <v>550</v>
       </c>
@@ -3690,7 +3690,7 @@
         <v>5.0623052959501562</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="48" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" ht="46" x14ac:dyDescent="0.35">
       <c r="A25" s="30" t="s">
         <v>551</v>
       </c>
@@ -3738,7 +3738,7 @@
         <v>29.984423676012465</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="24" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" ht="23" x14ac:dyDescent="0.35">
       <c r="A26" s="30" t="s">
         <v>552</v>
       </c>
@@ -3786,7 +3786,7 @@
         <v>1.7912772585669781</v>
       </c>
     </row>
-    <row r="27" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" ht="57.5" x14ac:dyDescent="0.35">
       <c r="A27" s="30" t="s">
         <v>553</v>
       </c>
@@ -3834,7 +3834,7 @@
         <v>2.1806853582554515</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" ht="57.5" x14ac:dyDescent="0.35">
       <c r="A28" s="30" t="s">
         <v>554</v>
       </c>
@@ -3882,7 +3882,7 @@
         <v>65.420560747663544</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A29" s="30" t="s">
         <v>555</v>
       </c>
@@ -3924,7 +3924,7 @@
         <v>3.0373831775700939</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="72" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" ht="69" x14ac:dyDescent="0.35">
       <c r="A30" s="30" t="s">
         <v>647</v>
       </c>
@@ -3972,7 +3972,7 @@
         <v>13.629283489096574</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="24" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A31" s="30" t="s">
         <v>556</v>
       </c>
@@ -4020,7 +4020,7 @@
         <v>5.8411214953271031</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A32" s="30" t="s">
         <v>557</v>
       </c>
@@ -4068,7 +4068,7 @@
         <v>19.080996884735203</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A33" s="30" t="s">
         <v>558</v>
       </c>
@@ -4103,12 +4103,12 @@
       <c r="N33" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="O33" s="33">
+      <c r="O33" s="33" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" ht="36" x14ac:dyDescent="0.25">
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="1:15" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A34" s="30" t="s">
         <v>559</v>
       </c>
@@ -4156,7 +4156,7 @@
         <v>11.292834890965734</v>
       </c>
     </row>
-    <row r="35" spans="1:15" ht="24" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" ht="23" x14ac:dyDescent="0.35">
       <c r="A35" s="30" t="s">
         <v>560</v>
       </c>
@@ -4198,7 +4198,7 @@
         <v>6.230529595015577</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A36" s="30" t="s">
         <v>561</v>
       </c>
@@ -4240,7 +4240,7 @@
         <v>1.0903426791277258</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A37" s="30" t="s">
         <v>562</v>
       </c>
@@ -4288,7 +4288,7 @@
         <v>7.3987538940809969</v>
       </c>
     </row>
-    <row r="38" spans="1:15" ht="24" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" ht="23" x14ac:dyDescent="0.35">
       <c r="A38" s="30" t="s">
         <v>563</v>
       </c>
@@ -4323,12 +4323,12 @@
       <c r="N38" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="O38" s="33">
+      <c r="O38" s="33" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+        <v/>
+      </c>
+    </row>
+    <row r="39" spans="1:15" ht="57.5" x14ac:dyDescent="0.35">
       <c r="A39" s="30" t="s">
         <v>564</v>
       </c>
@@ -4376,7 +4376,7 @@
         <v>52.18068535825546</v>
       </c>
     </row>
-    <row r="40" spans="1:15" ht="24" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" ht="23" x14ac:dyDescent="0.35">
       <c r="A40" s="30" t="s">
         <v>565</v>
       </c>
@@ -4424,7 +4424,7 @@
         <v>3.8161993769470413</v>
       </c>
     </row>
-    <row r="41" spans="1:15" ht="24" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" ht="23" x14ac:dyDescent="0.35">
       <c r="A41" s="30" t="s">
         <v>566</v>
       </c>
@@ -4466,7 +4466,7 @@
         <v>1.5965732087227413</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A42" s="30" t="s">
         <v>567</v>
       </c>
@@ -4514,7 +4514,7 @@
         <v>6.61993769470405</v>
       </c>
     </row>
-    <row r="43" spans="1:15" ht="36" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A43" s="30" t="s">
         <v>568</v>
       </c>
@@ -4556,7 +4556,7 @@
         <v>7.009345794392523</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A44" s="30" t="s">
         <v>569</v>
       </c>
@@ -4598,7 +4598,7 @@
         <v>5.0623052959501562</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A45" s="30" t="s">
         <v>570</v>
       </c>
@@ -4633,12 +4633,12 @@
       <c r="N45" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="O45" s="33">
+      <c r="O45" s="33" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+        <v/>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A46" s="30" t="s">
         <v>571</v>
       </c>
@@ -4686,7 +4686,7 @@
         <v>8.5669781931464168</v>
       </c>
     </row>
-    <row r="47" spans="1:15" ht="36" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A47" s="30" t="s">
         <v>572</v>
       </c>
@@ -4734,7 +4734,7 @@
         <v>10.124610591900312</v>
       </c>
     </row>
-    <row r="48" spans="1:15" ht="72" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" ht="69" x14ac:dyDescent="0.35">
       <c r="A48" s="30" t="s">
         <v>573</v>
       </c>
@@ -4782,7 +4782,7 @@
         <v>35.046728971962622</v>
       </c>
     </row>
-    <row r="49" spans="1:15" ht="24" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" ht="23" x14ac:dyDescent="0.35">
       <c r="A49" s="30" t="s">
         <v>574</v>
       </c>
@@ -4824,7 +4824,7 @@
         <v>10.514018691588786</v>
       </c>
     </row>
-    <row r="50" spans="1:15" ht="36" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A50" s="30" t="s">
         <v>575</v>
       </c>
@@ -4866,7 +4866,7 @@
         <v>13.629283489096574</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A51" s="30" t="s">
         <v>576</v>
       </c>
@@ -4908,7 +4908,7 @@
         <v>52.9595015576324</v>
       </c>
     </row>
-    <row r="52" spans="1:15" ht="36" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A52" s="30" t="s">
         <v>577</v>
       </c>
@@ -4956,7 +4956,7 @@
         <v>4.6728971962616832</v>
       </c>
     </row>
-    <row r="53" spans="1:15" ht="24" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" ht="23" x14ac:dyDescent="0.35">
       <c r="A53" s="30" t="s">
         <v>578</v>
       </c>
@@ -5004,7 +5004,7 @@
         <v>5.8411214953271031</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A54" s="30" t="s">
         <v>579</v>
       </c>
@@ -5046,7 +5046,7 @@
         <v>3.0373831775700939</v>
       </c>
     </row>
-    <row r="55" spans="1:15" ht="24" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" ht="23" x14ac:dyDescent="0.35">
       <c r="A55" s="30" t="s">
         <v>580</v>
       </c>
@@ -5094,7 +5094,7 @@
         <v>5.0623052959501562</v>
       </c>
     </row>
-    <row r="56" spans="1:15" ht="24" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" ht="23" x14ac:dyDescent="0.35">
       <c r="A56" s="30" t="s">
         <v>581</v>
       </c>
@@ -5142,7 +5142,7 @@
         <v>0.7398753894080996</v>
       </c>
     </row>
-    <row r="57" spans="1:15" ht="24" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" ht="23" x14ac:dyDescent="0.35">
       <c r="A57" s="30" t="s">
         <v>582</v>
       </c>
@@ -5190,7 +5190,7 @@
         <v>34.657320872274148</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A58" s="30" t="s">
         <v>583</v>
       </c>
@@ -5225,12 +5225,12 @@
       <c r="N58" s="7" t="s">
         <v>267</v>
       </c>
-      <c r="O58" s="33">
+      <c r="O58" s="33" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:15" ht="24" x14ac:dyDescent="0.25">
+        <v/>
+      </c>
+    </row>
+    <row r="59" spans="1:15" ht="23" x14ac:dyDescent="0.35">
       <c r="A59" s="30" t="s">
         <v>584</v>
       </c>
@@ -5265,12 +5265,12 @@
       <c r="N59" s="7" t="s">
         <v>271</v>
       </c>
-      <c r="O59" s="33">
+      <c r="O59" s="33" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+        <v/>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A60" s="30" t="s">
         <v>585</v>
       </c>
@@ -5305,12 +5305,12 @@
       <c r="N60" s="7" t="s">
         <v>276</v>
       </c>
-      <c r="O60" s="33">
+      <c r="O60" s="33" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+        <v/>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A61" s="30" t="s">
         <v>586</v>
       </c>
@@ -5345,12 +5345,12 @@
       <c r="N61" s="7" t="s">
         <v>281</v>
       </c>
-      <c r="O61" s="33">
+      <c r="O61" s="33" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:15" ht="36" x14ac:dyDescent="0.25">
+        <v/>
+      </c>
+    </row>
+    <row r="62" spans="1:15" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A62" s="30" t="s">
         <v>587</v>
       </c>
@@ -5398,7 +5398,7 @@
         <v>5.4517133956386301</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A63" s="30" t="s">
         <v>588</v>
       </c>
@@ -5440,7 +5440,7 @@
         <v>2.5700934579439254</v>
       </c>
     </row>
-    <row r="64" spans="1:15" ht="36" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A64" s="30" t="s">
         <v>589</v>
       </c>
@@ -5488,7 +5488,7 @@
         <v>6.230529595015577</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A65" s="30" t="s">
         <v>590</v>
       </c>
@@ -5536,7 +5536,7 @@
         <v>5.8411214953271031</v>
       </c>
     </row>
-    <row r="66" spans="1:15" ht="72" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:15" ht="69" x14ac:dyDescent="0.35">
       <c r="A66" s="30" t="s">
         <v>591</v>
       </c>
@@ -5584,7 +5584,7 @@
         <v>16.355140186915886</v>
       </c>
     </row>
-    <row r="67" spans="1:15" ht="24" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15" ht="23" x14ac:dyDescent="0.35">
       <c r="A67" s="30" t="s">
         <v>592</v>
       </c>
@@ -5622,11 +5622,11 @@
       <c r="M67" s="14"/>
       <c r="N67" s="14"/>
       <c r="O67" s="33">
-        <f t="shared" ref="O67:O119" si="1">K67/120/21.4*1000</f>
+        <f t="shared" ref="O67:O119" si="1">IF(NOT(ISBLANK(K67)),K67/120/21.4*1000,"")</f>
         <v>29.595015576323988</v>
       </c>
     </row>
-    <row r="68" spans="1:15" ht="24" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:15" ht="23" x14ac:dyDescent="0.35">
       <c r="A68" s="30" t="s">
         <v>593</v>
       </c>
@@ -5674,7 +5674,7 @@
         <v>3.1931464174454827</v>
       </c>
     </row>
-    <row r="69" spans="1:15" ht="72" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15" ht="69" x14ac:dyDescent="0.35">
       <c r="A69" s="30" t="s">
         <v>594</v>
       </c>
@@ -5722,7 +5722,7 @@
         <v>65.031152647975091</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A70" s="30" t="s">
         <v>595</v>
       </c>
@@ -5764,7 +5764,7 @@
         <v>17.912772585669785</v>
       </c>
     </row>
-    <row r="71" spans="1:15" ht="24" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15" ht="23" x14ac:dyDescent="0.35">
       <c r="A71" s="30" t="s">
         <v>596</v>
       </c>
@@ -5812,7 +5812,7 @@
         <v>26.4797507788162</v>
       </c>
     </row>
-    <row r="72" spans="1:15" ht="36" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:15" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A72" s="30" t="s">
         <v>597</v>
       </c>
@@ -5860,7 +5860,7 @@
         <v>23.364485981308412</v>
       </c>
     </row>
-    <row r="73" spans="1:15" ht="24" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:15" ht="23" x14ac:dyDescent="0.35">
       <c r="A73" s="30" t="s">
         <v>598</v>
       </c>
@@ -5895,12 +5895,12 @@
       <c r="N73" s="7" t="s">
         <v>334</v>
       </c>
-      <c r="O73" s="33">
+      <c r="O73" s="33" t="str">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+        <v/>
+      </c>
+    </row>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A74" s="30" t="s">
         <v>599</v>
       </c>
@@ -5942,7 +5942,7 @@
         <v>12.07165109034268</v>
       </c>
     </row>
-    <row r="75" spans="1:15" ht="24" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:15" ht="23" x14ac:dyDescent="0.35">
       <c r="A75" s="30" t="s">
         <v>600</v>
       </c>
@@ -5990,7 +5990,7 @@
         <v>3.2710280373831782</v>
       </c>
     </row>
-    <row r="76" spans="1:15" ht="48" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:15" ht="46" x14ac:dyDescent="0.35">
       <c r="A76" s="30" t="s">
         <v>601</v>
       </c>
@@ -6032,7 +6032,7 @@
         <v>1.4018691588785048</v>
       </c>
     </row>
-    <row r="77" spans="1:15" ht="24" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:15" ht="23" x14ac:dyDescent="0.35">
       <c r="A77" s="30" t="s">
         <v>602</v>
       </c>
@@ -6074,7 +6074,7 @@
         <v>4.6728971962616832</v>
       </c>
     </row>
-    <row r="78" spans="1:15" ht="36" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:15" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A78" s="30" t="s">
         <v>603</v>
       </c>
@@ -6116,7 +6116,7 @@
         <v>3.2710280373831782</v>
       </c>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A79" s="30" t="s">
         <v>604</v>
       </c>
@@ -6158,7 +6158,7 @@
         <v>4.2834890965732084</v>
       </c>
     </row>
-    <row r="80" spans="1:15" ht="36" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:15" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A80" s="30" t="s">
         <v>605</v>
       </c>
@@ -6206,7 +6206,7 @@
         <v>9.3457943925233664</v>
       </c>
     </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A81" s="30" t="s">
         <v>606</v>
       </c>
@@ -6248,7 +6248,7 @@
         <v>0.81775700934579454</v>
       </c>
     </row>
-    <row r="82" spans="1:15" ht="24" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:15" ht="23" x14ac:dyDescent="0.35">
       <c r="A82" s="30" t="s">
         <v>607</v>
       </c>
@@ -6290,7 +6290,7 @@
         <v>2.5311526479750781</v>
       </c>
     </row>
-    <row r="83" spans="1:15" ht="48" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:15" ht="46" x14ac:dyDescent="0.35">
       <c r="A83" s="30" t="s">
         <v>608</v>
       </c>
@@ -6338,7 +6338,7 @@
         <v>3.3489096573208728</v>
       </c>
     </row>
-    <row r="84" spans="1:15" ht="36" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:15" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A84" s="30" t="s">
         <v>609</v>
       </c>
@@ -6380,7 +6380,7 @@
         <v>5.8411214953271031</v>
       </c>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A85" s="30" t="s">
         <v>610</v>
       </c>
@@ -6415,12 +6415,12 @@
       <c r="N85" s="7" t="s">
         <v>383</v>
       </c>
-      <c r="O85" s="33">
+      <c r="O85" s="33" t="str">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:15" ht="24" x14ac:dyDescent="0.25">
+        <v/>
+      </c>
+    </row>
+    <row r="86" spans="1:15" ht="23" x14ac:dyDescent="0.35">
       <c r="A86" s="30" t="s">
         <v>611</v>
       </c>
@@ -6468,7 +6468,7 @@
         <v>5.4517133956386301</v>
       </c>
     </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A87" s="30" t="s">
         <v>612</v>
       </c>
@@ -6516,7 +6516,7 @@
         <v>22.585669781931468</v>
       </c>
     </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A88" s="30" t="s">
         <v>613</v>
       </c>
@@ -6564,7 +6564,7 @@
         <v>41.277258566978198</v>
       </c>
     </row>
-    <row r="89" spans="1:15" ht="24" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:15" ht="23" x14ac:dyDescent="0.35">
       <c r="A89" s="30" t="s">
         <v>614</v>
       </c>
@@ -6612,7 +6612,7 @@
         <v>38.940809968847354</v>
       </c>
     </row>
-    <row r="90" spans="1:15" ht="72" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:15" ht="69" x14ac:dyDescent="0.35">
       <c r="A90" s="30" t="s">
         <v>615</v>
       </c>
@@ -6660,7 +6660,7 @@
         <v>19.470404984423677</v>
       </c>
     </row>
-    <row r="91" spans="1:15" ht="24" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:15" ht="23" x14ac:dyDescent="0.35">
       <c r="A91" s="30" t="s">
         <v>616</v>
       </c>
@@ -6708,7 +6708,7 @@
         <v>7.3987538940809969</v>
       </c>
     </row>
-    <row r="92" spans="1:15" ht="24" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:15" ht="23" x14ac:dyDescent="0.35">
       <c r="A92" s="30" t="s">
         <v>617</v>
       </c>
@@ -6756,7 +6756,7 @@
         <v>8.9563862928348925</v>
       </c>
     </row>
-    <row r="93" spans="1:15" ht="36" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:15" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A93" s="30" t="s">
         <v>618</v>
       </c>
@@ -6804,7 +6804,7 @@
         <v>6.61993769470405</v>
       </c>
     </row>
-    <row r="94" spans="1:15" ht="36" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:15" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A94" s="30" t="s">
         <v>619</v>
       </c>
@@ -6846,7 +6846,7 @@
         <v>1.32398753894081</v>
       </c>
     </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A95" s="30" t="s">
         <v>620</v>
       </c>
@@ -6881,12 +6881,12 @@
       <c r="N95" s="7" t="s">
         <v>426</v>
       </c>
-      <c r="O95" s="33">
+      <c r="O95" s="33" t="str">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
+        <v/>
+      </c>
+    </row>
+    <row r="96" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A96" s="30" t="s">
         <v>621</v>
       </c>
@@ -6921,12 +6921,12 @@
       <c r="N96" s="7" t="s">
         <v>430</v>
       </c>
-      <c r="O96" s="33">
+      <c r="O96" s="33" t="str">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="1:15" ht="24" x14ac:dyDescent="0.25">
+        <v/>
+      </c>
+    </row>
+    <row r="97" spans="1:15" ht="23" x14ac:dyDescent="0.35">
       <c r="A97" s="30" t="s">
         <v>622</v>
       </c>
@@ -6974,7 +6974,7 @@
         <v>10.90342679127726</v>
       </c>
     </row>
-    <row r="98" spans="1:15" ht="24" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:15" ht="23" x14ac:dyDescent="0.35">
       <c r="A98" s="30" t="s">
         <v>623</v>
       </c>
@@ -7016,7 +7016,7 @@
         <v>8.5669781931464168</v>
       </c>
     </row>
-    <row r="99" spans="1:15" ht="24" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:15" ht="23" x14ac:dyDescent="0.35">
       <c r="A99" s="30" t="s">
         <v>624</v>
       </c>
@@ -7051,12 +7051,12 @@
       <c r="N99" s="7" t="s">
         <v>442</v>
       </c>
-      <c r="O99" s="33">
+      <c r="O99" s="33" t="str">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
+        <v/>
+      </c>
+    </row>
+    <row r="100" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A100" s="30" t="s">
         <v>625</v>
       </c>
@@ -7091,12 +7091,12 @@
       <c r="N100" s="7" t="s">
         <v>446</v>
       </c>
-      <c r="O100" s="33">
+      <c r="O100" s="33" t="str">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
+        <v/>
+      </c>
+    </row>
+    <row r="101" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A101" s="30" t="s">
         <v>626</v>
       </c>
@@ -7138,7 +7138,7 @@
         <v>7.3987538940809969</v>
       </c>
     </row>
-    <row r="102" spans="1:15" ht="36" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:15" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A102" s="30" t="s">
         <v>627</v>
       </c>
@@ -7186,7 +7186,7 @@
         <v>9.3457943925233664</v>
       </c>
     </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A103" s="30" t="s">
         <v>628</v>
       </c>
@@ -7228,7 +7228,7 @@
         <v>2.4143302180685362</v>
       </c>
     </row>
-    <row r="104" spans="1:15" ht="24" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:15" ht="23" x14ac:dyDescent="0.35">
       <c r="A104" s="30" t="s">
         <v>629</v>
       </c>
@@ -7263,12 +7263,12 @@
       <c r="N104" s="7" t="s">
         <v>461</v>
       </c>
-      <c r="O104" s="33">
+      <c r="O104" s="33" t="str">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
+        <v/>
+      </c>
+    </row>
+    <row r="105" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A105" s="30" t="s">
         <v>630</v>
       </c>
@@ -7310,7 +7310,7 @@
         <v>2.3364485981308416</v>
       </c>
     </row>
-    <row r="106" spans="1:15" ht="24" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:15" ht="23" x14ac:dyDescent="0.35">
       <c r="A106" s="30" t="s">
         <v>631</v>
       </c>
@@ -7358,7 +7358,7 @@
         <v>1.8691588785046729</v>
       </c>
     </row>
-    <row r="107" spans="1:15" ht="24" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:15" ht="23" x14ac:dyDescent="0.35">
       <c r="A107" s="30" t="s">
         <v>632</v>
       </c>
@@ -7406,7 +7406,7 @@
         <v>0.77881619937694713</v>
       </c>
     </row>
-    <row r="108" spans="1:15" ht="24" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:15" ht="23" x14ac:dyDescent="0.35">
       <c r="A108" s="30" t="s">
         <v>633</v>
       </c>
@@ -7448,7 +7448,7 @@
         <v>3.8161993769470413</v>
       </c>
     </row>
-    <row r="109" spans="1:15" ht="36" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:15" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A109" s="30" t="s">
         <v>634</v>
       </c>
@@ -7496,7 +7496,7 @@
         <v>1.32398753894081</v>
       </c>
     </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A110" s="30" t="s">
         <v>635</v>
       </c>
@@ -7544,7 +7544,7 @@
         <v>7.3987538940809969</v>
       </c>
     </row>
-    <row r="111" spans="1:15" ht="24" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:15" ht="23" x14ac:dyDescent="0.35">
       <c r="A111" s="30" t="s">
         <v>636</v>
       </c>
@@ -7592,7 +7592,7 @@
         <v>2.4922118380062313</v>
       </c>
     </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A112" s="30" t="s">
         <v>637</v>
       </c>
@@ -7640,7 +7640,7 @@
         <v>58.411214953271035</v>
       </c>
     </row>
-    <row r="113" spans="1:15" ht="72" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:15" ht="69" x14ac:dyDescent="0.35">
       <c r="A113" s="30" t="s">
         <v>638</v>
       </c>
@@ -7688,7 +7688,7 @@
         <v>41.277258566978198</v>
       </c>
     </row>
-    <row r="114" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A114" s="30" t="s">
         <v>639</v>
       </c>
@@ -7736,7 +7736,7 @@
         <v>1.1682242990654208</v>
       </c>
     </row>
-    <row r="115" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A115" s="32" t="s">
         <v>640</v>
       </c>
@@ -7778,7 +7778,7 @@
         <v>1.0514018691588787</v>
       </c>
     </row>
-    <row r="116" spans="1:15" ht="24" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:15" ht="23" x14ac:dyDescent="0.35">
       <c r="A116" s="30" t="s">
         <v>641</v>
       </c>
@@ -7820,7 +7820,7 @@
         <v>2.8426791277258565</v>
       </c>
     </row>
-    <row r="117" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A117" s="30" t="s">
         <v>642</v>
       </c>
@@ -7862,7 +7862,7 @@
         <v>2.4143302180685362</v>
       </c>
     </row>
-    <row r="118" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A118" s="30" t="s">
         <v>643</v>
       </c>
@@ -7904,7 +7904,7 @@
         <v>2.2975077881619943</v>
       </c>
     </row>
-    <row r="119" spans="1:15" ht="36" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:15" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A119" s="30" t="s">
         <v>644</v>
       </c>

</xml_diff>